<commit_message>
Actualizacion 2025/04/24 modulo update hc evemed
</commit_message>
<xml_diff>
--- a/ActividadesProyecto.xlsx
+++ b/ActividadesProyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julio\Documents\Personal\Proyectos\PlataformaSalud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8A52FF-D750-4F01-AF94-D4CAB08C2B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F70C79-1BB4-4233-BEFC-EE68E8681C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{5A375E53-5F29-42EA-B55E-8F0EAC125E90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5A375E53-5F29-42EA-B55E-8F0EAC125E90}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555BB51E-AD34-4A39-91E5-23D041F65CA2}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +754,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="9"/>
     </row>
@@ -767,21 +767,21 @@
       </c>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>12</v>
+      <c r="B16" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="9"/>
     </row>
@@ -861,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B72D22-1882-4B0C-958D-EA30A3CFCAC3}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>